<commit_message>
sibling match and updated va index regs to fix missing values
Created siblingmatch.do and uniquefamily.do to match siblings conditional on same year and link all siblings across years in the same family, respectively. Also updated VA regs on index and controls to fix discrepancy of observation numbers between imputed bivariate and imputed with controls. Discrepancy due to missing values in elprop
</commit_message>
<xml_diff>
--- a/out/xls/factoranalysis/categoryindex/compcase/clean_vaindex_compregs_all.xlsx
+++ b/out/xls/factoranalysis/categoryindex/compcase/clean_vaindex_compregs_all.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Dropbox\Davis\Research Projects\Ed Lab GSR\caschls\out\xls\factoranalysis\categoryindex\compcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F361337-A5B6-4AE8-BE85-932D789FDD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9FB4A5-9D45-46FA-BD3E-2FFAFE24F287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="9570" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="55">
   <si>
     <t>Value Added Variables</t>
   </si>
@@ -178,6 +178,27 @@
   </si>
   <si>
     <t>Counseling Support</t>
+  </si>
+  <si>
+    <t>392</t>
+  </si>
+  <si>
+    <t>384</t>
+  </si>
+  <si>
+    <t>288</t>
+  </si>
+  <si>
+    <t>284</t>
+  </si>
+  <si>
+    <t>374</t>
+  </si>
+  <si>
+    <t>370</t>
+  </si>
+  <si>
+    <t>369</t>
   </si>
 </sst>
 </file>
@@ -535,7 +556,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -710,47 +731,47 @@
       <c r="A7" t="s">
         <v>31</v>
       </c>
-      <c r="B7">
-        <v>309</v>
-      </c>
-      <c r="C7">
-        <v>309</v>
-      </c>
-      <c r="D7">
-        <v>304</v>
-      </c>
-      <c r="E7">
-        <v>304</v>
-      </c>
-      <c r="F7">
-        <v>304</v>
-      </c>
-      <c r="G7">
-        <v>304</v>
-      </c>
-      <c r="H7">
-        <v>304</v>
-      </c>
-      <c r="I7">
-        <v>304</v>
-      </c>
-      <c r="J7">
-        <v>304</v>
-      </c>
-      <c r="K7">
-        <v>304</v>
-      </c>
-      <c r="L7">
-        <v>304</v>
-      </c>
-      <c r="M7">
-        <v>304</v>
-      </c>
-      <c r="N7">
-        <v>304</v>
-      </c>
-      <c r="O7">
-        <v>304</v>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" t="s">
+        <v>49</v>
+      </c>
+      <c r="O7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
@@ -848,47 +869,47 @@
       <c r="A10" t="s">
         <v>31</v>
       </c>
-      <c r="B10">
-        <v>307</v>
-      </c>
-      <c r="C10">
-        <v>307</v>
-      </c>
-      <c r="D10">
-        <v>303</v>
-      </c>
-      <c r="E10">
-        <v>303</v>
-      </c>
-      <c r="F10">
-        <v>303</v>
-      </c>
-      <c r="G10">
-        <v>303</v>
-      </c>
-      <c r="H10">
-        <v>303</v>
-      </c>
-      <c r="I10">
-        <v>303</v>
-      </c>
-      <c r="J10">
-        <v>303</v>
-      </c>
-      <c r="K10">
-        <v>303</v>
-      </c>
-      <c r="L10">
-        <v>303</v>
-      </c>
-      <c r="M10">
-        <v>303</v>
-      </c>
-      <c r="N10">
-        <v>303</v>
-      </c>
-      <c r="O10">
-        <v>303</v>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L10" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10" t="s">
+        <v>51</v>
+      </c>
+      <c r="N10" t="s">
+        <v>51</v>
+      </c>
+      <c r="O10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
@@ -986,47 +1007,47 @@
       <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c r="B13">
-        <v>374</v>
-      </c>
-      <c r="C13">
-        <v>374</v>
-      </c>
-      <c r="D13">
-        <v>370</v>
-      </c>
-      <c r="E13">
-        <v>369</v>
-      </c>
-      <c r="F13">
-        <v>369</v>
-      </c>
-      <c r="G13">
-        <v>369</v>
-      </c>
-      <c r="H13">
-        <v>370</v>
-      </c>
-      <c r="I13">
-        <v>369</v>
-      </c>
-      <c r="J13">
-        <v>369</v>
-      </c>
-      <c r="K13">
-        <v>369</v>
-      </c>
-      <c r="L13">
-        <v>370</v>
-      </c>
-      <c r="M13">
-        <v>369</v>
-      </c>
-      <c r="N13">
-        <v>369</v>
-      </c>
-      <c r="O13">
-        <v>369</v>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" t="s">
+        <v>54</v>
+      </c>
+      <c r="J13" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L13" t="s">
+        <v>53</v>
+      </c>
+      <c r="M13" t="s">
+        <v>54</v>
+      </c>
+      <c r="N13" t="s">
+        <v>54</v>
+      </c>
+      <c r="O13" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">

</xml_diff>